<commit_message>
Added special cybernetic to the list
</commit_message>
<xml_diff>
--- a/RefsInterface/cybernetics_list.xlsx
+++ b/RefsInterface/cybernetics_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IMI\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IMI\RefsInterface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F793860C-73E8-4165-B019-9F5D3FE5A4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC755F0-82F9-4B22-AEF3-5E34A4A8E9F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{BB25BF14-BC81-40FB-93DA-055717F25838}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="567">
   <si>
     <t>Chipware Socket</t>
   </si>
@@ -1854,6 +1854,24 @@
   </si>
   <si>
     <t>The Bio-Borg. Grafted Muscle and/or Muscle &amp; Bone Lace, Speed Grafts, Neural Processor, Kerenzikov Boost R1 (+1/-0), Pain Editor, Biomonitor, Skinweave R5, Lifesaver Weave, Toxin Binders, Pacesetter 2000 heart, Rebreather Lungs, Nanoptical Rebuild (IR, LL).</t>
+  </si>
+  <si>
+    <t>Johnny Silverhand</t>
+  </si>
+  <si>
+    <t>Wake</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>fuck</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>Samurai</t>
   </si>
 </sst>
 </file>
@@ -2299,10 +2317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89ADA21-AF58-4DA1-8BA5-95E698C92F49}">
-  <dimension ref="A1:F247"/>
+  <dimension ref="A1:F248"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A248" sqref="A248"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3821,215 +3839,215 @@
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C78" s="2">
         <v>1750</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E77" s="2">
-        <v>2</v>
-      </c>
-      <c r="F77" s="1" t="s">
+      <c r="E78" s="2">
+        <v>2</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:6" ht="70" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" s="2">
+      <c r="B79" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="2">
         <v>4000</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E78" s="2">
-        <v>2</v>
-      </c>
-      <c r="F78" s="1" t="s">
+      <c r="E79" s="2">
+        <v>2</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C80" s="2">
         <v>15000</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E80" s="2">
         <v>5</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C81" s="2">
         <v>500</v>
       </c>
-      <c r="D80" s="2">
-        <v>3</v>
-      </c>
-      <c r="E80" s="2">
-        <v>2</v>
-      </c>
-      <c r="F80" s="1" t="s">
+      <c r="D81" s="2">
+        <v>3</v>
+      </c>
+      <c r="E81" s="2">
+        <v>2</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C81" s="2" t="s">
+      <c r="B82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D81" s="2">
-        <v>3</v>
-      </c>
-      <c r="E81" s="3">
+      <c r="D82" s="2">
+        <v>3</v>
+      </c>
+      <c r="E82" s="3">
         <v>43865</v>
       </c>
-      <c r="F81" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" s="2">
+      <c r="B83" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="2">
         <v>400</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E82" s="2">
-        <v>3</v>
-      </c>
-      <c r="F82" s="1" t="s">
+      <c r="E83" s="2">
+        <v>3</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="2">
+      <c r="B84" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="2">
         <v>750</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E83" s="2">
-        <v>2</v>
-      </c>
-      <c r="F83" s="1" t="s">
+      <c r="D84" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" s="2">
+        <v>2</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:6" ht="70" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C85" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E85" s="2">
         <v>6</v>
       </c>
-      <c r="F84" s="1" t="s">
+      <c r="F85" s="1" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C85" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E85" s="2">
-        <v>3</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C86" s="2">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="E86" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C87" s="2">
-        <v>3500</v>
+        <v>1500</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>3</v>
@@ -4038,48 +4056,48 @@
         <v>4</v>
       </c>
       <c r="F87" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" s="2">
+        <v>3500</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E88" s="2">
+        <v>4</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:6" ht="70" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C88" s="2" t="s">
+      <c r="B89" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="1" t="s">
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C89" s="2">
-        <v>3000</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E89" s="2">
-        <v>4</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>12</v>
@@ -4094,12 +4112,12 @@
         <v>4</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>12</v>
@@ -4114,12 +4132,12 @@
         <v>4</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>12</v>
@@ -4134,298 +4152,298 @@
         <v>4</v>
       </c>
       <c r="F92" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93" s="2">
+        <v>4</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:6" ht="70" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="2" t="s">
+      <c r="B94" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E93" s="3">
+      <c r="D94" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94" s="3">
         <v>43896</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="F94" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C94" s="2">
+      <c r="B95" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95" s="2">
         <v>100</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D95" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E94" s="2">
-        <v>3</v>
-      </c>
-      <c r="F94" s="1" t="s">
+      <c r="E95" s="2">
+        <v>3</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C95" s="2">
+      <c r="B96" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C96" s="2">
         <v>200</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E95" s="2">
-        <v>3</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" s="2">
-        <v>400</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E96" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C97" s="2">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>229</v>
+        <v>59</v>
       </c>
       <c r="E97" s="2">
         <v>4</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C98" s="2">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>85</v>
+        <v>229</v>
       </c>
       <c r="E98" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" s="2">
+        <v>400</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E99" s="2">
+        <v>3</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C99" s="2">
+      <c r="B100" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="2">
         <v>700</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="D100" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="E99" s="2">
-        <v>4</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C100" s="2">
-        <v>1200</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="E100" s="2">
         <v>4</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C101" s="2">
-        <v>850</v>
+        <v>1200</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>59</v>
+        <v>236</v>
       </c>
       <c r="E101" s="2">
         <v>4</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="C102" s="2">
-        <v>1200</v>
+        <v>850</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>241</v>
+        <v>59</v>
       </c>
       <c r="E102" s="2">
         <v>4</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C103" s="2">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E103" s="2">
         <v>4</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C104" s="2">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E104" s="2">
         <v>4</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" s="2">
+        <v>400</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E105" s="2">
+        <v>4</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C105" s="2">
+      <c r="B106" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="2">
         <v>1000</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E105" s="2">
+      <c r="E106" s="2">
         <v>5</v>
       </c>
-      <c r="F105" s="1" t="s">
+      <c r="F106" s="1" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A106" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C106" s="2">
-        <v>400</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E106" s="2">
-        <v>4</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C107" s="2">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>236</v>
@@ -4434,124 +4452,124 @@
         <v>4</v>
       </c>
       <c r="F107" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="2">
+        <v>700</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E108" s="2">
+        <v>4</v>
+      </c>
+      <c r="F108" s="1" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A108" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C108" s="2">
-        <v>500</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E108" s="2">
-        <v>2</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C109" s="2">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="E109" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="C110" s="2">
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>260</v>
+        <v>59</v>
       </c>
       <c r="E110" s="2">
         <v>3</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C111" s="2">
+        <v>750</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E111" s="2">
+        <v>3</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C111" s="2">
+      <c r="C112" s="2">
         <v>1200</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="D112" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E111" s="2">
-        <v>3</v>
-      </c>
-      <c r="F111" s="1" t="s">
+      <c r="E112" s="2">
+        <v>3</v>
+      </c>
+      <c r="F112" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A112" s="5" t="s">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A113" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="2"/>
-      <c r="E112" s="2"/>
-      <c r="F112" s="5" t="s">
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="5" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A113" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C113" s="2">
-        <v>300</v>
-      </c>
-      <c r="D113" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E113" s="2">
-        <v>2</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>12</v>
@@ -4560,98 +4578,98 @@
         <v>300</v>
       </c>
       <c r="D114" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E114" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F114" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C115" s="2">
+        <v>300</v>
+      </c>
+      <c r="D115" s="2">
+        <v>1</v>
+      </c>
+      <c r="E115" s="2">
+        <v>3</v>
+      </c>
+      <c r="F115" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C115" s="2">
+      <c r="B116" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C116" s="2">
         <v>200</v>
       </c>
-      <c r="D115" s="2">
-        <v>2</v>
-      </c>
-      <c r="E115" s="2">
+      <c r="D116" s="2">
+        <v>2</v>
+      </c>
+      <c r="E116" s="2">
         <v>4</v>
       </c>
-      <c r="F115" s="1" t="s">
+      <c r="F116" s="1" t="s">
         <v>272</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A116" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C116" s="2">
-        <v>300</v>
-      </c>
-      <c r="D116" s="2">
-        <v>1</v>
-      </c>
-      <c r="E116" s="2">
-        <v>2</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C117" s="2">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D117" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E117" s="2">
         <v>2</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C118" s="2">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="D118" s="2">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E118" s="2">
         <v>2</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>12</v>
@@ -4666,18 +4684,18 @@
         <v>2</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C120" s="2">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="D120" s="2">
         <v>0.5</v>
@@ -4686,12 +4704,12 @@
         <v>2</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>12</v>
@@ -4706,12 +4724,12 @@
         <v>2</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>12</v>
@@ -4720,18 +4738,18 @@
         <v>200</v>
       </c>
       <c r="D122" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E122" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>12</v>
@@ -4746,12 +4764,12 @@
         <v>3</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>12</v>
@@ -4766,32 +4784,32 @@
         <v>3</v>
       </c>
       <c r="F124" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C125" s="2">
+        <v>200</v>
+      </c>
+      <c r="D125" s="2">
+        <v>1</v>
+      </c>
+      <c r="E125" s="2">
+        <v>3</v>
+      </c>
+      <c r="F125" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A125" s="1" t="s">
+    <row r="126" spans="1:6" ht="56" x14ac:dyDescent="0.35">
+      <c r="A126" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C125" s="2">
-        <v>300</v>
-      </c>
-      <c r="D125" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E125" s="2">
-        <v>2</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A126" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>12</v>
@@ -4806,52 +4824,52 @@
         <v>2</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="42" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C127" s="2">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D127" s="2">
         <v>0.5</v>
       </c>
       <c r="E127" s="2">
+        <v>2</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C128" s="2">
+        <v>200</v>
+      </c>
+      <c r="D128" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E128" s="2">
         <v>4</v>
       </c>
-      <c r="F127" s="1" t="s">
+      <c r="F128" s="1" t="s">
         <v>296</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A128" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C128" s="2">
-        <v>350</v>
-      </c>
-      <c r="D128" s="2">
-        <v>1</v>
-      </c>
-      <c r="E128" s="2">
-        <v>3</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>12</v>
@@ -4860,338 +4878,338 @@
         <v>350</v>
       </c>
       <c r="D129" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E129" s="2">
         <v>3</v>
       </c>
       <c r="F129" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130" s="2">
+        <v>350</v>
+      </c>
+      <c r="D130" s="2">
+        <v>2</v>
+      </c>
+      <c r="E130" s="2">
+        <v>3</v>
+      </c>
+      <c r="F130" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A130" s="1" t="s">
+    <row r="131" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A131" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C130" s="2">
+      <c r="B131" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C131" s="2">
         <v>200</v>
       </c>
-      <c r="D130" s="2">
-        <v>2</v>
-      </c>
-      <c r="E130" s="2">
-        <v>3</v>
-      </c>
-      <c r="F130" s="1" t="s">
+      <c r="D131" s="2">
+        <v>2</v>
+      </c>
+      <c r="E131" s="2">
+        <v>3</v>
+      </c>
+      <c r="F131" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A131" s="1" t="s">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C131" s="2">
+      <c r="C132" s="2">
         <v>1500</v>
       </c>
-      <c r="D131" s="2" t="s">
+      <c r="D132" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E131" s="2">
-        <v>2</v>
-      </c>
-      <c r="F131" s="1" t="s">
+      <c r="E132" s="2">
+        <v>2</v>
+      </c>
+      <c r="F132" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A132" s="1" t="s">
+    <row r="133" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A133" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C132" s="2">
+      <c r="B133" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C133" s="2">
         <v>300</v>
       </c>
-      <c r="D132" s="2">
-        <v>1</v>
-      </c>
-      <c r="E132" s="2">
-        <v>2</v>
-      </c>
-      <c r="F132" s="1" t="s">
+      <c r="D133" s="2">
+        <v>1</v>
+      </c>
+      <c r="E133" s="2">
+        <v>2</v>
+      </c>
+      <c r="F133" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A133" s="1" t="s">
+    <row r="134" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A134" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C133" s="2">
+      <c r="B134" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" s="2">
         <v>425</v>
       </c>
-      <c r="D133" s="2">
-        <v>1</v>
-      </c>
-      <c r="E133" s="2">
-        <v>3</v>
-      </c>
-      <c r="F133" s="1" t="s">
+      <c r="D134" s="2">
+        <v>1</v>
+      </c>
+      <c r="E134" s="2">
+        <v>3</v>
+      </c>
+      <c r="F134" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A134" s="1" t="s">
+    <row r="135" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A135" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B135" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C134" s="2">
+      <c r="C135" s="2">
         <v>600</v>
       </c>
-      <c r="D134" s="2" t="s">
+      <c r="D135" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E134" s="2">
-        <v>2</v>
-      </c>
-      <c r="F134" s="1" t="s">
+      <c r="E135" s="2">
+        <v>2</v>
+      </c>
+      <c r="F135" s="1" t="s">
         <v>311</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A135" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C135" s="2">
-        <v>400</v>
-      </c>
-      <c r="D135" s="2">
-        <v>1</v>
-      </c>
-      <c r="E135" s="2">
-        <v>2</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C136" s="2">
-        <v>750</v>
+        <v>400</v>
       </c>
       <c r="D136" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E136" s="2">
         <v>2</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" s="2">
+        <v>750</v>
+      </c>
+      <c r="D137" s="2">
+        <v>3</v>
+      </c>
+      <c r="E137" s="2">
+        <v>2</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C137" s="2">
+      <c r="B138" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138" s="2">
         <v>1000</v>
       </c>
-      <c r="D137" s="2">
+      <c r="D138" s="2">
         <v>5</v>
       </c>
-      <c r="E137" s="2">
-        <v>2</v>
-      </c>
-      <c r="F137" s="1" t="s">
+      <c r="E138" s="2">
+        <v>2</v>
+      </c>
+      <c r="F138" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A138" s="1" t="s">
+    <row r="139" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A139" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C138" s="2">
-        <v>2000</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E138" s="2">
-        <v>3</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A139" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C139" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E139" s="2">
+        <v>3</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C140" s="2">
         <v>500</v>
       </c>
-      <c r="D139" s="2" t="s">
+      <c r="D140" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E139" s="2">
-        <v>2</v>
-      </c>
-      <c r="F139" s="1" t="s">
+      <c r="E140" s="2">
+        <v>2</v>
+      </c>
+      <c r="F140" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A140" s="1" t="s">
+    <row r="141" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C140" s="2">
+      <c r="B141" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C141" s="2">
         <v>200</v>
       </c>
-      <c r="D140" s="2">
-        <v>1</v>
-      </c>
-      <c r="E140" s="2">
-        <v>2</v>
-      </c>
-      <c r="F140" s="1" t="s">
+      <c r="D141" s="2">
+        <v>1</v>
+      </c>
+      <c r="E141" s="2">
+        <v>2</v>
+      </c>
+      <c r="F141" s="1" t="s">
         <v>324</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A141" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C141" s="2">
-        <v>100</v>
-      </c>
-      <c r="D141" s="2">
-        <v>1</v>
-      </c>
-      <c r="E141" s="2">
-        <v>2</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C142" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D142" s="2">
         <v>1</v>
       </c>
       <c r="E142" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C143" s="2">
+        <v>500</v>
+      </c>
+      <c r="D143" s="2">
+        <v>1</v>
+      </c>
+      <c r="E143" s="2">
+        <v>4</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B143" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C143" s="2">
+      <c r="B144" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C144" s="2">
         <v>100</v>
       </c>
-      <c r="D143" s="2">
+      <c r="D144" s="2">
         <v>0</v>
       </c>
-      <c r="E143" s="2">
-        <v>2</v>
-      </c>
-      <c r="F143" s="1" t="s">
+      <c r="E144" s="2">
+        <v>2</v>
+      </c>
+      <c r="F144" s="1" t="s">
         <v>330</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A144" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C144" s="2">
-        <v>150</v>
-      </c>
-      <c r="D144" s="2">
-        <v>1</v>
-      </c>
-      <c r="E144" s="2">
-        <v>2</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C145" s="2">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="D145" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E145" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>12</v>
@@ -5200,84 +5218,84 @@
         <v>200</v>
       </c>
       <c r="D146" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E146" s="2">
         <v>3</v>
       </c>
       <c r="F146" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A147" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C147" s="2">
+        <v>200</v>
+      </c>
+      <c r="D147" s="2">
+        <v>1</v>
+      </c>
+      <c r="E147" s="2">
+        <v>3</v>
+      </c>
+      <c r="F147" s="1" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A147" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C147" s="2">
-        <v>350</v>
-      </c>
-      <c r="D147" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E147" s="2">
-        <v>3</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C148" s="2">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="D148" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E148" s="2">
         <v>3</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C149" s="2">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D149" s="2">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E149" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C150" s="2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D150" s="2">
         <v>0.5</v>
@@ -5286,12 +5304,12 @@
         <v>2</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>12</v>
@@ -5303,15 +5321,15 @@
         <v>0.5</v>
       </c>
       <c r="E151" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>12</v>
@@ -5323,15 +5341,15 @@
         <v>0.5</v>
       </c>
       <c r="E152" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>12</v>
@@ -5340,18 +5358,18 @@
         <v>200</v>
       </c>
       <c r="D153" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E153" s="2">
         <v>4</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>12</v>
@@ -5360,44 +5378,44 @@
         <v>200</v>
       </c>
       <c r="D154" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E154" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F154" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C155" s="2">
+        <v>200</v>
+      </c>
+      <c r="D155" s="2">
+        <v>2</v>
+      </c>
+      <c r="E155" s="2">
+        <v>3</v>
+      </c>
+      <c r="F155" s="1" t="s">
         <v>352</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A155" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C155" s="2">
-        <v>100</v>
-      </c>
-      <c r="D155" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E155" s="2">
-        <v>2</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C156" s="2">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D156" s="2">
         <v>0.5</v>
@@ -5406,72 +5424,72 @@
         <v>2</v>
       </c>
       <c r="F156" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C157" s="2">
+        <v>300</v>
+      </c>
+      <c r="D157" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E157" s="2">
+        <v>2</v>
+      </c>
+      <c r="F157" s="1" t="s">
         <v>356</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A157" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C157" s="2">
-        <v>220</v>
-      </c>
-      <c r="D157" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E157" s="2">
-        <v>3</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>122</v>
+        <v>12</v>
       </c>
       <c r="C158" s="2">
-        <v>3000</v>
+        <v>220</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="E158" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C159" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>241</v>
+        <v>85</v>
       </c>
       <c r="E159" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>122</v>
@@ -5480,98 +5498,98 @@
         <v>4000</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>85</v>
+        <v>241</v>
       </c>
       <c r="E160" s="2">
         <v>3</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C161" s="2">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E161" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C162" s="2" t="s">
-        <v>368</v>
+      <c r="C162" s="2">
+        <v>2000</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>369</v>
+        <v>85</v>
       </c>
       <c r="E162" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E163" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C164" s="2">
-        <v>200</v>
+        <v>122</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>372</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E164" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>12</v>
@@ -5579,119 +5597,119 @@
       <c r="C165" s="2">
         <v>200</v>
       </c>
-      <c r="D165" s="2">
-        <v>3</v>
+      <c r="D165" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="E165" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C166" s="2">
+        <v>200</v>
+      </c>
+      <c r="D166" s="2">
+        <v>3</v>
+      </c>
+      <c r="E166" s="2">
+        <v>2</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A167" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B166" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C166" s="2">
+      <c r="B167" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C167" s="2">
         <v>300</v>
       </c>
-      <c r="D166" s="2">
-        <v>2</v>
-      </c>
-      <c r="E166" s="2">
-        <v>3</v>
-      </c>
-      <c r="F166" s="1" t="s">
+      <c r="D167" s="2">
+        <v>2</v>
+      </c>
+      <c r="E167" s="2">
+        <v>3</v>
+      </c>
+      <c r="F167" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A167" s="1" t="s">
+    <row r="168" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A168" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B168" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C167" s="2">
+      <c r="C168" s="2">
         <v>1500</v>
       </c>
-      <c r="D167" s="2" t="s">
+      <c r="D168" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E167" s="2">
-        <v>3</v>
-      </c>
-      <c r="F167" s="1" t="s">
+      <c r="E168" s="2">
+        <v>3</v>
+      </c>
+      <c r="F168" s="1" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A168" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C168" s="2">
-        <v>300</v>
-      </c>
-      <c r="D168" s="2">
-        <v>1</v>
-      </c>
-      <c r="E168" s="2">
-        <v>3</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C169" s="2">
+        <v>300</v>
+      </c>
+      <c r="D169" s="2">
+        <v>1</v>
+      </c>
+      <c r="E169" s="2">
+        <v>3</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A170" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B169" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C169" s="2" t="s">
+      <c r="B170" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C170" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D169" s="2">
-        <v>1</v>
-      </c>
-      <c r="E169" s="2">
-        <v>2</v>
-      </c>
-      <c r="F169" s="1" t="s">
+      <c r="D170" s="2">
+        <v>1</v>
+      </c>
+      <c r="E170" s="2">
+        <v>2</v>
+      </c>
+      <c r="F170" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A170" s="1" t="s">
+    <row r="171" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A171" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C170" s="2">
-        <v>200</v>
-      </c>
-      <c r="D170" s="2">
-        <v>0</v>
-      </c>
-      <c r="E170" s="2">
-        <v>2</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A171" s="1" t="s">
-        <v>390</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>12</v>
@@ -5700,18 +5718,18 @@
         <v>200</v>
       </c>
       <c r="D171" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E171" s="2">
         <v>2</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>12</v>
@@ -5720,18 +5738,18 @@
         <v>200</v>
       </c>
       <c r="D172" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E172" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>12</v>
@@ -5740,64 +5758,64 @@
         <v>200</v>
       </c>
       <c r="D173" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E173" s="2">
         <v>3</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C174" s="2">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="D174" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E174" s="2">
         <v>3</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C175" s="2">
+        <v>350</v>
+      </c>
+      <c r="D175" s="2">
+        <v>1</v>
+      </c>
+      <c r="E175" s="2">
+        <v>3</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A176" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="B175" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C175" s="2">
+      <c r="B176" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C176" s="2">
         <v>800</v>
-      </c>
-      <c r="D175" s="2">
-        <v>0</v>
-      </c>
-      <c r="E175" s="2">
-        <v>3</v>
-      </c>
-      <c r="F175" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A176" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>401</v>
       </c>
       <c r="D176" s="2">
         <v>0</v>
@@ -5806,112 +5824,112 @@
         <v>3</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C177" s="2">
-        <v>500</v>
-      </c>
-      <c r="D177" s="2" t="s">
-        <v>66</v>
+      <c r="C177" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D177" s="2">
+        <v>0</v>
       </c>
       <c r="E177" s="2">
         <v>3</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C178" s="2">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E178" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F178" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A179" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C179" s="2">
+        <v>200</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E179" s="2">
+        <v>2</v>
+      </c>
+      <c r="F179" s="1" t="s">
         <v>406</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A179" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C179" s="2">
-        <v>600</v>
-      </c>
-      <c r="D179" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E179" s="2">
-        <v>3</v>
-      </c>
-      <c r="F179" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C180" s="2">
-        <v>300</v>
-      </c>
-      <c r="D180" s="2">
-        <v>2</v>
+        <v>600</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E180" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C181" s="2">
+        <v>300</v>
+      </c>
+      <c r="D181" s="2">
+        <v>2</v>
+      </c>
+      <c r="E181" s="2">
+        <v>2</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A182" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C181" s="2">
-        <v>500</v>
-      </c>
-      <c r="D181" s="2">
-        <v>2</v>
-      </c>
-      <c r="E181" s="2">
-        <v>2</v>
-      </c>
-      <c r="F181" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A182" s="1" t="s">
-        <v>413</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>12</v>
@@ -5926,78 +5944,78 @@
         <v>2</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C183" s="2">
+        <v>500</v>
+      </c>
+      <c r="D183" s="2">
+        <v>2</v>
+      </c>
+      <c r="E183" s="2">
+        <v>2</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A184" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B183" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C183" s="2">
+      <c r="B184" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C184" s="2">
         <v>450</v>
       </c>
-      <c r="D183" s="2" t="s">
+      <c r="D184" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E183" s="2">
-        <v>2</v>
-      </c>
-      <c r="F183" s="1" t="s">
+      <c r="E184" s="2">
+        <v>2</v>
+      </c>
+      <c r="F184" s="1" t="s">
         <v>416</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A184" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C184" s="2">
-        <v>500</v>
-      </c>
-      <c r="D184" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E184" s="2">
-        <v>4</v>
-      </c>
-      <c r="F184" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C185" s="2">
-        <v>150</v>
-      </c>
-      <c r="D185" s="2">
-        <v>1</v>
+        <v>500</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E185" s="2">
         <v>4</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C186" s="2">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="D186" s="2">
         <v>1</v>
@@ -6006,158 +6024,158 @@
         <v>4</v>
       </c>
       <c r="F186" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A187" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C187" s="2">
+        <v>250</v>
+      </c>
+      <c r="D187" s="2">
+        <v>1</v>
+      </c>
+      <c r="E187" s="2">
+        <v>4</v>
+      </c>
+      <c r="F187" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A187" s="1" t="s">
+    <row r="188" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A188" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B187" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C187" s="2" t="s">
+      <c r="B188" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C188" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="D187" s="2">
-        <v>1</v>
-      </c>
-      <c r="E187" s="2">
-        <v>2</v>
-      </c>
-      <c r="F187" s="1" t="s">
+      <c r="D188" s="2">
+        <v>1</v>
+      </c>
+      <c r="E188" s="2">
+        <v>2</v>
+      </c>
+      <c r="F188" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A188" s="1" t="s">
+    <row r="189" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A189" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B188" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C188" s="2">
+      <c r="B189" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C189" s="2">
         <v>1000</v>
       </c>
-      <c r="D188" s="2">
-        <v>1</v>
-      </c>
-      <c r="E188" s="2">
-        <v>2</v>
-      </c>
-      <c r="F188" s="1" t="s">
+      <c r="D189" s="2">
+        <v>1</v>
+      </c>
+      <c r="E189" s="2">
+        <v>2</v>
+      </c>
+      <c r="F189" s="1" t="s">
         <v>426</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A189" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C189" s="2">
-        <v>50</v>
-      </c>
-      <c r="D189" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E189" s="2">
-        <v>2</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C190" s="2">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="D190" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E190" s="2">
         <v>2</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C191" s="2">
+        <v>500</v>
+      </c>
+      <c r="D191" s="2">
+        <v>2</v>
+      </c>
+      <c r="E191" s="2">
+        <v>2</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A192" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="B191" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C191" s="2">
+      <c r="B192" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C192" s="2">
         <v>200</v>
       </c>
-      <c r="D191" s="2">
-        <v>2</v>
-      </c>
-      <c r="E191" s="2">
-        <v>2</v>
-      </c>
-      <c r="F191" s="1" t="s">
+      <c r="D192" s="2">
+        <v>2</v>
+      </c>
+      <c r="E192" s="2">
+        <v>2</v>
+      </c>
+      <c r="F192" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A192" s="1" t="s">
+    <row r="193" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A193" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B192" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C192" s="2">
+      <c r="B193" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C193" s="2">
         <v>100</v>
       </c>
-      <c r="D192" s="2">
-        <v>1</v>
-      </c>
-      <c r="E192" s="2">
-        <v>3</v>
-      </c>
-      <c r="F192" s="1" t="s">
+      <c r="D193" s="2">
+        <v>1</v>
+      </c>
+      <c r="E193" s="2">
+        <v>3</v>
+      </c>
+      <c r="F193" s="1" t="s">
         <v>434</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A193" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C193" s="2">
-        <v>200</v>
-      </c>
-      <c r="D193" s="2">
-        <v>1</v>
-      </c>
-      <c r="E193" s="2">
-        <v>2</v>
-      </c>
-      <c r="F193" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C194" s="2">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D194" s="2">
         <v>1</v>
@@ -6166,72 +6184,72 @@
         <v>2</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C195" s="2">
+        <v>180</v>
+      </c>
+      <c r="D195" s="2">
+        <v>1</v>
+      </c>
+      <c r="E195" s="2">
+        <v>2</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A196" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="B195" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C195" s="2" t="s">
+      <c r="B196" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C196" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="D195" s="2">
-        <v>1</v>
-      </c>
-      <c r="E195" s="2">
+      <c r="D196" s="2">
+        <v>1</v>
+      </c>
+      <c r="E196" s="2">
         <v>4</v>
       </c>
-      <c r="F195" s="1" t="s">
+      <c r="F196" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A196" s="1" t="s">
+    <row r="197" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A197" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="B196" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C196" s="2">
+      <c r="B197" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C197" s="2">
         <v>500</v>
       </c>
-      <c r="D196" s="2" t="s">
+      <c r="D197" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E196" s="2">
-        <v>3</v>
-      </c>
-      <c r="F196" s="1" t="s">
+      <c r="E197" s="2">
+        <v>3</v>
+      </c>
+      <c r="F197" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A197" s="1" t="s">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A198" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C197" s="2">
-        <v>200</v>
-      </c>
-      <c r="D197" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E197" s="2">
-        <v>2</v>
-      </c>
-      <c r="F197" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A198" s="1" t="s">
-        <v>446</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>12</v>
@@ -6239,339 +6257,339 @@
       <c r="C198" s="2">
         <v>200</v>
       </c>
-      <c r="D198" s="2">
+      <c r="D198" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E198" s="2">
+        <v>2</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A199" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C199" s="2">
+        <v>200</v>
+      </c>
+      <c r="D199" s="2">
         <v>0</v>
       </c>
-      <c r="E198" s="2">
+      <c r="E199" s="2">
         <v>4</v>
       </c>
-      <c r="F198" s="1" t="s">
+      <c r="F199" s="1" t="s">
         <v>447</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A199" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C199" s="2">
-        <v>500</v>
-      </c>
-      <c r="D199" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E199" s="2">
-        <v>6</v>
-      </c>
-      <c r="F199" s="1" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C200" s="2">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E200" s="2" t="s">
-        <v>451</v>
+      <c r="E200" s="2">
+        <v>6</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C201" s="2" t="s">
-        <v>114</v>
+      <c r="C201" s="2">
+        <v>1500</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C202" s="2">
-        <v>600</v>
+      <c r="C202" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E202" s="2">
+      <c r="E202" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A203" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C203" s="2">
+        <v>600</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E203" s="2">
         <v>5</v>
       </c>
-      <c r="F202" s="1" t="s">
+      <c r="F203" s="1" t="s">
         <v>457</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A203" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="B203" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C203" s="2">
-        <v>200</v>
-      </c>
-      <c r="D203" s="2">
-        <v>3</v>
-      </c>
-      <c r="E203" s="2">
-        <v>4</v>
-      </c>
-      <c r="F203" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C204" s="2">
-        <v>800</v>
-      </c>
-      <c r="D204" s="2" t="s">
-        <v>85</v>
+        <v>200</v>
+      </c>
+      <c r="D204" s="2">
+        <v>3</v>
       </c>
       <c r="E204" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C205" s="2">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="E205" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C206" s="2">
+        <v>400</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E206" s="2">
+        <v>4</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A207" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B206" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C206" s="2">
+      <c r="B207" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C207" s="2">
         <v>475</v>
       </c>
-      <c r="D206" s="2" t="s">
+      <c r="D207" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E206" s="2">
-        <v>3</v>
-      </c>
-      <c r="F206" s="1" t="s">
+      <c r="E207" s="2">
+        <v>3</v>
+      </c>
+      <c r="F207" s="1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A207" s="1" t="s">
+    <row r="208" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A208" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B207" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C207" s="2">
+      <c r="B208" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C208" s="2">
         <v>275</v>
       </c>
-      <c r="D207" s="2" t="s">
+      <c r="D208" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E207" s="2">
-        <v>3</v>
-      </c>
-      <c r="F207" s="1" t="s">
+      <c r="E208" s="2">
+        <v>3</v>
+      </c>
+      <c r="F208" s="1" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A208" s="1" t="s">
+    <row r="209" spans="1:6" ht="56" x14ac:dyDescent="0.35">
+      <c r="A209" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="B208" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C208" s="2">
+      <c r="B209" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C209" s="2">
         <v>250</v>
       </c>
-      <c r="D208" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E208" s="2">
-        <v>3</v>
-      </c>
-      <c r="F208" s="1" t="s">
+      <c r="D209" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E209" s="2">
+        <v>3</v>
+      </c>
+      <c r="F209" s="1" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A209" s="1" t="s">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A210" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B209" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C209" s="2">
+      <c r="B210" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C210" s="2">
         <v>350</v>
       </c>
-      <c r="D209" s="2" t="s">
+      <c r="D210" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E209" s="2">
+      <c r="E210" s="2">
         <v>5</v>
       </c>
-      <c r="F209" s="1" t="s">
+      <c r="F210" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A210" s="1" t="s">
+    <row r="211" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A211" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="B210" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C210" s="2">
+      <c r="B211" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C211" s="2">
         <v>1250</v>
       </c>
-      <c r="D210" s="2" t="s">
+      <c r="D211" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="E210" s="2">
+      <c r="E211" s="2">
         <v>4</v>
       </c>
-      <c r="F210" s="1" t="s">
+      <c r="F211" s="1" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A211" s="1" t="s">
+    <row r="212" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A212" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B211" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C211" s="2">
+      <c r="B212" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C212" s="2">
         <v>5000</v>
       </c>
-      <c r="D211" s="2" t="s">
+      <c r="D212" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E211" s="2">
+      <c r="E212" s="2">
         <v>6</v>
       </c>
-      <c r="F211" s="1" t="s">
+      <c r="F212" s="1" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A212" s="1" t="s">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A213" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="B212" s="2" t="s">
+      <c r="B213" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C212" s="2">
+      <c r="C213" s="2">
         <v>750</v>
       </c>
-      <c r="D212" s="2" t="s">
+      <c r="D213" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E212" s="2">
-        <v>2</v>
-      </c>
-      <c r="F212" s="1" t="s">
+      <c r="E213" s="2">
+        <v>2</v>
+      </c>
+      <c r="F213" s="1" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A213" s="1" t="s">
+    <row r="214" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A214" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="B213" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C213" s="2" t="s">
+      <c r="B214" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C214" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D213" s="2" t="s">
+      <c r="D214" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E213" s="2">
-        <v>2</v>
-      </c>
-      <c r="F213" s="1" t="s">
+      <c r="E214" s="2">
+        <v>2</v>
+      </c>
+      <c r="F214" s="1" t="s">
         <v>480</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A214" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C214" s="2">
-        <v>600</v>
-      </c>
-      <c r="D214" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E214" s="2">
-        <v>3</v>
-      </c>
-      <c r="F214" s="1" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>12</v>
@@ -6583,135 +6601,135 @@
         <v>85</v>
       </c>
       <c r="E215" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C216" s="2">
-        <v>200</v>
-      </c>
-      <c r="D216" s="2">
-        <v>2</v>
+        <v>600</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E216" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C217" s="2">
+        <v>200</v>
+      </c>
+      <c r="D217" s="2">
+        <v>2</v>
+      </c>
+      <c r="E217" s="2">
+        <v>3</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A218" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="B217" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C217" s="2">
+      <c r="B218" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C218" s="2">
         <v>600</v>
       </c>
-      <c r="D217" s="2">
-        <v>2</v>
-      </c>
-      <c r="E217" s="2">
-        <v>2</v>
-      </c>
-      <c r="F217" s="1" t="s">
+      <c r="D218" s="2">
+        <v>2</v>
+      </c>
+      <c r="E218" s="2">
+        <v>2</v>
+      </c>
+      <c r="F218" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A218" s="1" t="s">
+    <row r="219" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A219" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="B218" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C218" s="2">
+      <c r="B219" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C219" s="2">
         <v>1000</v>
       </c>
-      <c r="D218" s="2" t="s">
+      <c r="D219" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E218" s="2">
-        <v>3</v>
-      </c>
-      <c r="F218" s="1" t="s">
+      <c r="E219" s="2">
+        <v>3</v>
+      </c>
+      <c r="F219" s="1" t="s">
         <v>490</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A219" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B219" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C219" s="2">
-        <v>250</v>
-      </c>
-      <c r="D219" s="2">
-        <v>2</v>
-      </c>
-      <c r="E219" s="2">
-        <v>2</v>
-      </c>
-      <c r="F219" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C220" s="2">
+        <v>250</v>
+      </c>
+      <c r="D220" s="2">
+        <v>2</v>
+      </c>
+      <c r="E220" s="2">
+        <v>2</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A221" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B220" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C220" s="2">
+      <c r="B221" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C221" s="2">
         <v>300</v>
       </c>
-      <c r="D220" s="2">
-        <v>3</v>
-      </c>
-      <c r="E220" s="2">
+      <c r="D221" s="2">
+        <v>3</v>
+      </c>
+      <c r="E221" s="2">
         <v>4</v>
       </c>
-      <c r="F220" s="1" t="s">
+      <c r="F221" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A221" s="1" t="s">
+    <row r="222" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A222" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="B221" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C221" s="2">
-        <v>975</v>
-      </c>
-      <c r="D221" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E221" s="2">
-        <v>3</v>
-      </c>
-      <c r="F221" s="1" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A222" s="1" t="s">
-        <v>497</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>12</v>
@@ -6720,98 +6738,98 @@
         <v>975</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E222" s="2">
         <v>3</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C223" s="2">
+        <v>975</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E223" s="2">
+        <v>3</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A224" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="B223" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C223" s="2">
+      <c r="B224" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C224" s="2">
         <v>500</v>
       </c>
-      <c r="D223" s="2">
-        <v>1</v>
-      </c>
-      <c r="E223" s="2">
-        <v>2</v>
-      </c>
-      <c r="F223" s="1" t="s">
+      <c r="D224" s="2">
+        <v>1</v>
+      </c>
+      <c r="E224" s="2">
+        <v>2</v>
+      </c>
+      <c r="F224" s="1" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A224" s="1" t="s">
+    <row r="225" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A225" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="B224" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C224" s="2">
+      <c r="B225" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C225" s="2">
         <v>750</v>
       </c>
-      <c r="D224" s="2">
-        <v>1</v>
-      </c>
-      <c r="E224" s="2">
-        <v>2</v>
-      </c>
-      <c r="F224" s="1" t="s">
+      <c r="D225" s="2">
+        <v>1</v>
+      </c>
+      <c r="E225" s="2">
+        <v>2</v>
+      </c>
+      <c r="F225" s="1" t="s">
         <v>502</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A225" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C225" s="2">
-        <v>100</v>
-      </c>
-      <c r="D225" s="2">
-        <v>2</v>
-      </c>
-      <c r="E225" s="2">
-        <v>3</v>
-      </c>
-      <c r="F225" s="1" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
-        <v>504</v>
+        <v>295</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C226" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D226" s="2">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E226" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>12</v>
@@ -6826,12 +6844,12 @@
         <v>2</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>12</v>
@@ -6846,12 +6864,12 @@
         <v>2</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>12</v>
@@ -6866,12 +6884,12 @@
         <v>2</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>12</v>
@@ -6886,346 +6904,366 @@
         <v>2</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C231" s="2">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="D231" s="2">
         <v>0.5</v>
       </c>
       <c r="E231" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C232" s="2">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="D232" s="2">
         <v>0.5</v>
       </c>
       <c r="E232" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B233" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C233" s="2">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="D233" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E233" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C234" s="2">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D234" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E234" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C235" s="2">
+        <v>50</v>
+      </c>
+      <c r="D235" s="2">
+        <v>1</v>
+      </c>
+      <c r="E235" s="2">
+        <v>2</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A236" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="B235" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C235" s="2">
+      <c r="B236" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C236" s="2">
         <v>150</v>
       </c>
-      <c r="D235" s="2">
-        <v>2</v>
-      </c>
-      <c r="E235" s="2">
-        <v>3</v>
-      </c>
-      <c r="F235" s="1" t="s">
+      <c r="D236" s="2">
+        <v>2</v>
+      </c>
+      <c r="E236" s="2">
+        <v>3</v>
+      </c>
+      <c r="F236" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A236" s="1" t="s">
+    <row r="237" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A237" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="B236" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C236" s="2">
+      <c r="B237" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C237" s="2">
         <v>60</v>
       </c>
-      <c r="D236" s="2">
+      <c r="D237" s="2">
         <v>0</v>
       </c>
-      <c r="E236" s="2">
-        <v>2</v>
-      </c>
-      <c r="F236" s="1" t="s">
+      <c r="E237" s="2">
+        <v>2</v>
+      </c>
+      <c r="F237" s="1" t="s">
         <v>525</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" ht="84" x14ac:dyDescent="0.35">
-      <c r="A237" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="B237" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C237" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="D237" s="2">
-        <v>2</v>
-      </c>
-      <c r="E237" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="F237" s="1" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="238" spans="1:6" ht="84" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="C238" s="4" t="s">
         <v>527</v>
       </c>
       <c r="D238" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E238" s="2" t="s">
         <v>528</v>
       </c>
       <c r="F238" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" ht="84" x14ac:dyDescent="0.35">
+      <c r="A239" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="D239" s="2">
+        <v>4</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="F239" s="1" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A239" s="1" t="s">
+    <row r="240" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A240" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="B239" s="2" t="s">
+      <c r="B240" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="C239" s="2">
+      <c r="C240" s="2">
         <v>3400</v>
       </c>
-      <c r="D239" s="2" t="s">
+      <c r="D240" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="E239" s="2">
-        <v>2</v>
-      </c>
-      <c r="F239" s="1" t="s">
+      <c r="E240" s="2">
+        <v>2</v>
+      </c>
+      <c r="F240" s="1" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A240" s="6" t="s">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A241" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="B240" s="8" t="s">
+      <c r="B241" s="8" t="s">
         <v>538</v>
       </c>
-      <c r="C240" s="8">
+      <c r="C241" s="8">
         <v>1400</v>
       </c>
-      <c r="D240" s="8" t="s">
+      <c r="D241" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="E240" s="8">
-        <v>2</v>
-      </c>
-      <c r="F240" s="10" t="s">
+      <c r="E241" s="8">
+        <v>2</v>
+      </c>
+      <c r="F241" s="10" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A241" s="7" t="s">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A242" s="7" t="s">
         <v>537</v>
       </c>
-      <c r="B241" s="9"/>
-      <c r="C241" s="9"/>
-      <c r="D241" s="9"/>
-      <c r="E241" s="9"/>
-      <c r="F241" s="11"/>
-    </row>
-    <row r="242" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A242" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="B242" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="C242" s="2">
-        <v>1250</v>
-      </c>
-      <c r="D242" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E242" s="2">
-        <v>2</v>
-      </c>
-      <c r="F242" s="1" t="s">
-        <v>543</v>
-      </c>
+      <c r="B242" s="9"/>
+      <c r="C242" s="9"/>
+      <c r="D242" s="9"/>
+      <c r="E242" s="9"/>
+      <c r="F242" s="11"/>
     </row>
     <row r="243" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>1</v>
+        <v>542</v>
       </c>
       <c r="C243" s="2">
-        <v>1000</v>
+        <v>1250</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="E243" s="2">
         <v>2</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="244" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C244" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D244" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E244" s="2">
+        <v>2</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="A245" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="B244" s="2" t="s">
+      <c r="B245" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="C244" s="2">
+      <c r="C245" s="2">
         <v>9000</v>
       </c>
-      <c r="D244" s="2" t="s">
+      <c r="D245" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="E244" s="2">
-        <v>3</v>
-      </c>
-      <c r="F244" s="1" t="s">
+      <c r="E245" s="2">
+        <v>3</v>
+      </c>
+      <c r="F245" s="1" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="245" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A245" s="1" t="s">
+    <row r="246" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A246" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="B245" s="2" t="s">
+      <c r="B246" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C245" s="2">
+      <c r="C246" s="2">
         <v>24500</v>
       </c>
-      <c r="D245" s="2" t="s">
+      <c r="D246" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="E245" s="2">
-        <v>4</v>
-      </c>
-      <c r="F245" s="1" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A246" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="B246" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="C246" s="2">
-        <v>21000</v>
-      </c>
-      <c r="D246" s="2" t="s">
-        <v>556</v>
       </c>
       <c r="E246" s="2">
         <v>4</v>
       </c>
       <c r="F246" s="1" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" ht="70" x14ac:dyDescent="0.35">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C247" s="2">
-        <v>20000</v>
+        <v>21000</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="E247" s="2">
         <v>4</v>
       </c>
       <c r="F247" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" ht="70" x14ac:dyDescent="0.35">
+      <c r="A248" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C248" s="2">
+        <v>20000</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E248" s="2">
+        <v>4</v>
+      </c>
+      <c r="F248" s="1" t="s">
         <v>560</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B240:B241"/>
-    <mergeCell ref="C240:C241"/>
-    <mergeCell ref="D240:D241"/>
-    <mergeCell ref="E240:E241"/>
-    <mergeCell ref="F240:F241"/>
+    <mergeCell ref="B241:B242"/>
+    <mergeCell ref="C241:C242"/>
+    <mergeCell ref="D241:D242"/>
+    <mergeCell ref="E241:E242"/>
+    <mergeCell ref="F241:F242"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>